<commit_message>
added the missing documents
</commit_message>
<xml_diff>
--- a/Process Analytics Course Materials 2023/advanced_datasets/3 Process and Product Design/Cement/CementComposition.xlsx
+++ b/Process Analytics Course Materials 2023/advanced_datasets/3 Process and Product Design/Cement/CementComposition.xlsx
@@ -1608,13 +1608,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{119336A3-CEF2-4CD8-B43D-C9FC3049DF35}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B1F8A7-2EFC-4602-AF8E-5C099E2FFD5F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA86F7BC-5E9B-46DE-AAFE-C42DD2D8DD97}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F268600A-E195-4B82-9518-EEF6BA6494FC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{439FA931-CD81-4B8A-B990-9684B7A97FA9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01745D7C-ACCD-45F2-88EB-517277448E32}"/>
 </file>
</xml_diff>